<commit_message>
hpc 2008r2 run at .net 4 4.5
</commit_message>
<xml_diff>
--- a/AsianOptions/AsianOptionPricingCSharpBehind.xlsx
+++ b/AsianOptions/AsianOptionPricingCSharpBehind.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\administrator.HPCSOWHAT\Desktop\FSharpWCF\AsianOptions\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="20475" windowHeight="9345" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14595" windowHeight="3030"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="24">
   <si>
     <t>Up</t>
   </si>
@@ -85,17 +90,25 @@
   </si>
   <si>
     <t>HN001</t>
+  </si>
+  <si>
+    <t>Service</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>AsianOptionsService</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -120,7 +133,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -128,7 +141,7 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -137,6 +150,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -211,11 +231,31 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=2.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="178F42DEB120E91418F19D69140CE775361271"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3651"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1138"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=2.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -227,24 +267,7 @@
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
   <ax:ocxPr ax:name="Sizel_cx" ax:value="3598"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1111"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=2.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="178F42DEB120E91418F19D69140CE775361271"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3651"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1085"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1164"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -254,7 +277,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=2.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="158BE8DF21E4C714044190A4147116CBA3A741"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="3C66731B4376C834B4C3978239559B59AFF1C3"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -278,7 +301,7 @@
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
   <ax:ocxPr ax:name="Sizel_cx" ax:value="3969"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1032"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1085"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -288,14 +311,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=2.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="3C66731B4376C834B4C3978239559B59AFF1C3"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="158BE8DF21E4C714044190A4147116CBA3A741"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
   <ax:ocxPr ax:name="Sizel_cx" ax:value="3995"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1005"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1111"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -384,13 +407,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="153629056"/>
-        <c:axId val="153630592"/>
+        <c:axId val="565233328"/>
+        <c:axId val="565233888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="153629056"/>
+        <c:axId val="565233328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -399,7 +421,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153630592"/>
+        <c:crossAx val="565233888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -407,7 +429,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153630592"/>
+        <c:axId val="565233888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -418,7 +440,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153629056"/>
+        <c:crossAx val="565233328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -467,7 +489,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -475,6 +497,24 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -508,7 +548,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -516,6 +556,24 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -554,7 +612,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -562,6 +620,24 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -595,7 +671,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -603,6 +679,24 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -636,7 +730,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -644,6 +738,24 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -732,7 +844,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -767,7 +879,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -979,11 +1091,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.140625" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
@@ -1066,10 +1178,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -1135,6 +1247,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -1142,8 +1255,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId4" name="_ActiveXWrapper2">
+        <control shapeId="1025" r:id="rId4" name="_ActiveXWrapper1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>790575</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>695325</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1025" r:id="rId4" name="_ActiveXWrapper1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1026" r:id="rId6" name="_ActiveXWrapper2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -1162,32 +1300,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId4" name="_ActiveXWrapper2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId6" name="_ActiveXWrapper1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>790575</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>695325</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1025" r:id="rId6" name="_ActiveXWrapper1"/>
+        <control shapeId="1026" r:id="rId6" name="_ActiveXWrapper2"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -1199,11 +1312,11 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.140625" customWidth="1"/>
     <col min="2" max="2" width="10.140625" customWidth="1"/>
@@ -1417,6 +1530,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -1424,27 +1538,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2049" r:id="rId4" name="_ActiveXWrapper1">
+        <control shapeId="2051" r:id="rId4" name="_ActiveXWrapper3">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
-                <xdr:colOff>219075</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
+                <xdr:colOff>228600</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>314325</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
+                <xdr:colOff>323850</xdr:colOff>
+                <xdr:row>20</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2049" r:id="rId4" name="_ActiveXWrapper1"/>
+        <control shapeId="2051" r:id="rId4" name="_ActiveXWrapper3"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -1474,27 +1588,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2051" r:id="rId8" name="_ActiveXWrapper3">
+        <control shapeId="2049" r:id="rId8" name="_ActiveXWrapper1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
-                <xdr:colOff>228600</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
+                <xdr:colOff>219075</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>323850</xdr:colOff>
-                <xdr:row>20</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>314325</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2051" r:id="rId8" name="_ActiveXWrapper3"/>
+        <control shapeId="2049" r:id="rId8" name="_ActiveXWrapper1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -1510,9 +1624,10 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <dataConsolidate/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>